<commit_message>
remove vdecl function, fix ast calls
</commit_message>
<xml_diff>
--- a/LL Parse Table.xlsx
+++ b/LL Parse Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madelinezechar/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madelinezechar/plt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB7D4EF6-7F8B-4C42-B1FE-30148AD20A65}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181F3D77-26BC-6D42-BF79-EC2D1C12451D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="13400" windowHeight="15020" xr2:uid="{B1C2E3BE-DF2C-D443-BB42-222E6F3FBEDA}"/>
+    <workbookView xWindow="-14980" yWindow="460" windowWidth="24460" windowHeight="15020" xr2:uid="{B1C2E3BE-DF2C-D443-BB42-222E6F3FBEDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="92">
   <si>
     <t>State</t>
   </si>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>Assign</t>
-  </si>
-  <si>
-    <t>LPAREN actuals_opt RP…</t>
   </si>
   <si>
     <t>plus</t>
@@ -664,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D707DC87-2D22-1647-A63B-6AB45DC63B7E}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -744,37 +741,37 @@
         <v>63</v>
       </c>
       <c r="Y1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z1" t="s">
         <v>65</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>66</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>67</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>68</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>69</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>70</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>71</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>72</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>73</v>
       </c>
-      <c r="AH1" t="s">
-        <v>74</v>
-      </c>
       <c r="AI1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">
@@ -1106,7 +1103,7 @@
         <v>39</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H18" t="s">
         <v>39</v>
@@ -1115,16 +1112,16 @@
         <v>39</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="T18" t="b">
         <v>1</v>
@@ -1133,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="X18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Y18" t="s">
         <v>39</v>
@@ -1173,42 +1170,40 @@
       <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="G19" s="1"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="Z19" s="1" t="s">
+      <c r="AA19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AA19" s="1" t="s">
+      <c r="AB19" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AB19" s="1" t="s">
+      <c r="AC19" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AC19" s="1" t="s">
+      <c r="AD19" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AD19" s="1" t="s">
+      <c r="AE19" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AE19" s="1" t="s">
+      <c r="AF19" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AF19" s="1" t="s">
+      <c r="AG19" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AG19" s="1" t="s">
+      <c r="AH19" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AH19" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="AI19" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>